<commit_message>
Testing change to oid spreadsheet
</commit_message>
<xml_diff>
--- a/OID Tracking Spreadsheet_Dental.xlsx
+++ b/OID Tracking Spreadsheet_Dental.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF63C8B4-C817-449E-A89C-31A2FDA6FE61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1EAA10-91A9-4DDE-AB6F-DD4D6E1AD0AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OID" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Published IG version</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1219,7 @@
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>2</v>
@@ -2237,6 +2240,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004033853A35F3BB4292F626290EF9887D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="068fc46fc11ee629178abc4f12c265d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="873fe923d70bef4d578e1cd567cc05e2" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2441,29 +2466,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF2B2395-CA91-4D00-99F3-0B6B7B6FC9ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA7E1DC5-CDB2-4E1F-A809-8744593EDDFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E6962B-502F-4A84-B72B-B3C6D1BB7A58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2483,32 +2514,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA7E1DC5-CDB2-4E1F-A809-8744593EDDFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF2B2395-CA91-4D00-99F3-0B6B7B6FC9ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added dental referral note and dental consult note
</commit_message>
<xml_diff>
--- a/OID Tracking Spreadsheet_Dental.xlsx
+++ b/OID Tracking Spreadsheet_Dental.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1EAA10-91A9-4DDE-AB6F-DD4D6E1AD0AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BAFCAC-DE22-493C-8833-2BC378858052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OID" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Dental Referral Note</t>
+  </si>
+  <si>
+    <t>Dental Consult Note</t>
   </si>
 </sst>
 </file>
@@ -795,7 +801,7 @@
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +894,7 @@
       </c>
       <c r="B2" s="31"/>
       <c r="D2" s="10" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>2</v>
@@ -922,7 +928,9 @@
         <v>14</v>
       </c>
       <c r="B3" s="22"/>
-      <c r="D3" s="29"/>
+      <c r="D3" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" s="29"/>
       <c r="G3" s="10" t="s">
         <v>2</v>
@@ -2240,6 +2248,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2250,15 +2267,6 @@
     </LCG_x0020_Document_x0020_Workflow>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2467,6 +2475,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA7E1DC5-CDB2-4E1F-A809-8744593EDDFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF2B2395-CA91-4D00-99F3-0B6B7B6FC9ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2482,14 +2498,6 @@
     <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA7E1DC5-CDB2-4E1F-A809-8744593EDDFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added root oids for templates
</commit_message>
<xml_diff>
--- a/OID Tracking Spreadsheet_Dental.xlsx
+++ b/OID Tracking Spreadsheet_Dental.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A733E1B-5AAF-4A5F-9636-52428F522190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53076152-B6CD-4C6C-9E91-15C0B45618F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2445" windowWidth="21600" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OID" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>Title</t>
   </si>
@@ -119,7 +119,38 @@
     <t>Dental Consult Note</t>
   </si>
   <si>
-    <t>TEST</t>
+    <t xml:space="preserve"> 
+ 2.16.840.1.113883.10.20.40.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ 2.16.840.1.113883.10.20.40
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ 2.16.840.1.113883.10.20.40.1.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.10.20.40.1.2 </t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.10.20.40.1.3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.10.20.40.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ 2.16.840.1.113883.10.20.40.1.1.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ 2.16.840.1.113883.10.20.40.1.1.2
+</t>
   </si>
 </sst>
 </file>
@@ -129,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +254,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -433,12 +470,16 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -811,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +861,7 @@
     <col min="1" max="1" width="44.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="45.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="4.42578125" style="8" customWidth="1"/>
     <col min="7" max="8" width="51.5703125" style="6" customWidth="1"/>
@@ -899,16 +940,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:20" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="32"/>
       <c r="D2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
+      <c r="E2" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>2</v>
@@ -934,7 +975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
@@ -942,7 +983,9 @@
       <c r="D3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="29"/>
+      <c r="E3" s="33" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="10" t="s">
         <v>2</v>
       </c>
@@ -998,12 +1041,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>2</v>
+      <c r="B5" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="29"/>
@@ -1022,9 +1065,7 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="B6" s="33"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="G6" s="3"/>
@@ -1045,9 +1086,12 @@
       <c r="S6" s="26"/>
       <c r="T6" s="18"/>
     </row>
-    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1066,12 +1110,12 @@
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
+      <c r="B8" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -1098,7 +1142,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -1123,7 +1167,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -1142,9 +1186,6 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="G11" s="10"/>
@@ -1166,7 +1207,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
@@ -1320,8 +1361,8 @@
       <c r="T19" s="18"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>30</v>
+      <c r="A20" s="31" t="s">
+        <v>2</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
@@ -2251,6 +2292,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -2260,19 +2302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004033853A35F3BB4292F626290EF9887D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="068fc46fc11ee629178abc4f12c265d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="873fe923d70bef4d578e1cd567cc05e2" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2477,6 +2506,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2487,26 +2529,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF2B2395-CA91-4D00-99F3-0B6B7B6FC9ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E6962B-502F-4A84-B72B-B3C6D1BB7A58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2528,6 +2550,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF2B2395-CA91-4D00-99F3-0B6B7B6FC9ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="4f7f0390-f43e-47d2-8c36-9d39eaba7d2e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4F7F0390-F43E-47D2-8C36-9D39EABA7D2E"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA7E1DC5-CDB2-4E1F-A809-8744593EDDFE}">
   <ds:schemaRefs>

</xml_diff>